<commit_message>
Update README.md and minor quality of life changes
</commit_message>
<xml_diff>
--- a/TracibilityandDefectSheet.xlsx
+++ b/TracibilityandDefectSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET-PlatformScience\SDET-PlatformScienceAssigment-HaiTran\SDET-PlatformScienceAssigmentAutomationSuite-HaiTran\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA322C6-0B85-4B74-937E-062B097AAB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE8A64A-5E4E-43A1-9AC6-13B158578C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{BD96FC05-A932-4CFC-B87D-C71FDB6351F9}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" activeTab="1" xr2:uid="{BD96FC05-A932-4CFC-B87D-C71FDB6351F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracibility Sheet" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>Requirements</t>
   </si>
@@ -263,6 +263,30 @@
   </si>
   <si>
     <t>Defects</t>
+  </si>
+  <si>
+    <t>Send a negative coordination (either x,y or both) as a coordiation for room size in the post request</t>
+  </si>
+  <si>
+    <t>Send a negative coordination (either x,y or both) as a coordiation for dirt patch in the post request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send a negative coordination that is smaller than -1 (either x,y or both) as a default hovering location </t>
+  </si>
+  <si>
+    <t>Send a coordination (either x,y or both) larger or smaller than the room size for dirt patch in the post request</t>
+  </si>
+  <si>
+    <t>Send a coordination (either x,y or both) larger or than the room size for the default hover position in the post request</t>
+  </si>
+  <si>
+    <t>Send a JSONArray of [x,y,z] rather than [x,y] on any of the coordination input</t>
+  </si>
+  <si>
+    <t>Perform the step outline by the service specification in the pdf. Repeat the above step but remove the dirt patches creation coordinates. The application still return 1 dirt patch</t>
+  </si>
+  <si>
+    <t>In the automation suite, if multiple feature get run, the application will eventually filled up with dirt patches and force the user to re-launch the docker to get a clean slate</t>
   </si>
 </sst>
 </file>
@@ -418,12 +442,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -440,11 +463,63 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -461,15 +536,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -479,82 +545,38 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF470726-669C-43D2-A4DD-AED0B9DD1066}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -887,420 +909,420 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="115.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="E2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="26"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="E4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="48"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="28"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="E7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="41"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="41"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="30"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="32"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="8" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="E12" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="32"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="8" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="32"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="8" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="32"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="E15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="33"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="8" t="s">
+      <c r="A16" s="40"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="34" t="s">
+      <c r="E16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="E19" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="36"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="18" t="s">
+      <c r="A20" s="42"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="E20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="36"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="18" t="s">
+      <c r="A21" s="42"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="E21" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="36"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="18" t="s">
+      <c r="A22" s="42"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="E22" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="37"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="18" t="s">
+      <c r="A23" s="43"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="E23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
+      <c r="E24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="1"/>
@@ -1319,16 +1341,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:B3"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1337,67 +1359,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D4F8E6-8986-4A63-A799-FDBEC4C8A520}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="37.83984375" customWidth="1"/>
     <col min="2" max="2" width="38.734375" customWidth="1"/>
+    <col min="3" max="3" width="28.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>